<commit_message>
Resolved conflict in datafile
</commit_message>
<xml_diff>
--- a/Adult - Multi Distractor/two-five analysis.xlsx
+++ b/Adult - Multi Distractor/two-five analysis.xlsx
@@ -853,6 +853,11 @@
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
+  <c:spPr>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
@@ -1184,7 +1189,7 @@
   <dimension ref="A1:G36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M24" sqref="M24"/>
+      <selection activeCell="L31" sqref="L31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>

</xml_diff>